<commit_message>
Updated the process main file with device testing procedures
</commit_message>
<xml_diff>
--- a/src/Connected Office Web Application-User Acceptance Testing/Data/Connected Office Test Data.xlsx
+++ b/src/Connected Office Web Application-User Acceptance Testing/Data/Connected Office Test Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacqui.Muller\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WORK_SCHOOL\CMPG_323\CMPG-323-Project-4-37016776\src\Connected Office Web Application-User Acceptance Testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAB8EEF-425E-42A8-A7F1-FF25847C778D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9FBF8E3-DC18-4855-B5A8-A4551C61004B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38700" yWindow="300" windowWidth="14295" windowHeight="15300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="1" r:id="rId1"/>
@@ -687,7 +687,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1128,7 +1128,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1161,16 +1161,16 @@
         <v>57</v>
       </c>
       <c r="B2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1178,16 +1178,16 @@
         <v>58</v>
       </c>
       <c r="B3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1195,16 +1195,16 @@
         <v>59</v>
       </c>
       <c r="B4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1212,16 +1212,16 @@
         <v>60</v>
       </c>
       <c r="B5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1229,16 +1229,16 @@
         <v>61</v>
       </c>
       <c r="B6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1246,16 +1246,16 @@
         <v>62</v>
       </c>
       <c r="B7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1263,16 +1263,16 @@
         <v>63</v>
       </c>
       <c r="B8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1280,16 +1280,16 @@
         <v>64</v>
       </c>
       <c r="B9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1297,16 +1297,16 @@
         <v>65</v>
       </c>
       <c r="B10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1314,16 +1314,16 @@
         <v>66</v>
       </c>
       <c r="B11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1331,16 +1331,16 @@
         <v>67</v>
       </c>
       <c r="B12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1348,16 +1348,16 @@
         <v>68</v>
       </c>
       <c r="B13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1365,16 +1365,16 @@
         <v>69</v>
       </c>
       <c r="B14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1382,16 +1382,16 @@
         <v>70</v>
       </c>
       <c r="B15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1399,16 +1399,16 @@
         <v>48</v>
       </c>
       <c r="B16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1416,16 +1416,16 @@
         <v>49</v>
       </c>
       <c r="B17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1433,16 +1433,16 @@
         <v>50</v>
       </c>
       <c r="B18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1450,16 +1450,16 @@
         <v>51</v>
       </c>
       <c r="B19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1467,16 +1467,16 @@
         <v>52</v>
       </c>
       <c r="B20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1484,16 +1484,16 @@
         <v>53</v>
       </c>
       <c r="B21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1501,16 +1501,16 @@
         <v>54</v>
       </c>
       <c r="B22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1518,16 +1518,16 @@
         <v>55</v>
       </c>
       <c r="B23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1535,16 +1535,16 @@
         <v>56</v>
       </c>
       <c r="B24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>